<commit_message>
Update 1p5. FuelCell1Motor, 1D Chassis example, FTP75, Real-Time
</commit_message>
<xml_diff>
--- a/Libraries/Event/sm_car_database_Maneuver.xlsx
+++ b/Libraries/Event/sm_car_database_Maneuver.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Event\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41936EE-E547-4CCE-8EED-D48545191B65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C871CA09-E3C0-47E8-B61B-500ACE9E7185}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="4320" windowWidth="21600" windowHeight="11430" tabRatio="954" xr2:uid="{87770AAC-9142-4F0B-A47A-9193DA8A8904}"/>
+    <workbookView xWindow="390" yWindow="825" windowWidth="26040" windowHeight="11430" tabRatio="954" firstSheet="35" activeTab="44" xr2:uid="{87770AAC-9142-4F0B-A47A-9193DA8A8904}"/>
   </bookViews>
   <sheets>
     <sheet name="Mallory_HambaLG" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,8 @@
     <sheet name="RDF_Rough_HambaLG" sheetId="11" r:id="rId42"/>
     <sheet name="RDF_Rough_Hamba" sheetId="18" r:id="rId43"/>
     <sheet name="RDF_Rough_Makhulu" sheetId="27" r:id="rId44"/>
-    <sheet name="None" sheetId="29" r:id="rId45"/>
+    <sheet name="DriveCycle_FTP75" sheetId="50" r:id="rId45"/>
+    <sheet name="None" sheetId="29" r:id="rId46"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -75,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="80">
   <si>
     <t>m/s</t>
   </si>
@@ -304,6 +307,18 @@
   <si>
     <t>Scales target speed Trajectory vx</t>
   </si>
+  <si>
+    <t>DriveCycle</t>
+  </si>
+  <si>
+    <t>DriveCycle_FTP75.mat</t>
+  </si>
+  <si>
+    <t>DriveCycle_LoadFile</t>
+  </si>
+  <si>
+    <t>FTP75</t>
+  </si>
 </sst>
 </file>
 
@@ -464,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -519,12 +534,29 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="296">
+  <dxfs count="298">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -20006,12 +20038,12 @@
   </sheetPr>
   <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M35" sqref="M35"/>
       <selection pane="topRight" activeCell="M35" sqref="M35"/>
       <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20462,37 +20494,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="295" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="294" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="293" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="292" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="294" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="291" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="290" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="289" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20963,37 +20995,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="235" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="234" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="233" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="232" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="231" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="230" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="229" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21464,37 +21496,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="228" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="227" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="226" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="225" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="224" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="223" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="222" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21965,37 +21997,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="221" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="220" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="219" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="218" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="217" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="216" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="215" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22466,37 +22498,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="214" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="213" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="212" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="211" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="210" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="209" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="208" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22967,37 +22999,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="207" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="206" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="205" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="204" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="203" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23468,37 +23500,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="200" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="199" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="198" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="197" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="196" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="195" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="194" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23969,37 +24001,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="193" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="192" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="191" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="190" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="189" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="188" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="187" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24470,37 +24502,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="186" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="185" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="184" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="183" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="182" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="181" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24971,37 +25003,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="179" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="178" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="177" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="176" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="175" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="174" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="173" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25472,37 +25504,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="172" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="171" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="170" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="169" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="168" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="167" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="166" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25973,37 +26005,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="288" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="287" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="286" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="285" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="284" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="283" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="285" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="282" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26474,37 +26506,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="165" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="164" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="163" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="162" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="161" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="160" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="159" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26973,37 +27005,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="158" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="157" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="156" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="155" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="154" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="153" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="152" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27474,37 +27506,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="151" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="149" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="148" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="147" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="146" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="145" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27975,37 +28007,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="144" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="143" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="142" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="141" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="140" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="139" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="138" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28476,37 +28508,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="137" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="136" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="135" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="134" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="133" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="132" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="131" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28977,37 +29009,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="130" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="129" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="127" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="126" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="125" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="124" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29478,37 +29510,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="123" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="122" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="121" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="120" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="119" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="118" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="117" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30143,32 +30175,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="116" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="115" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="114" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="113" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="112" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="111" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30804,32 +30836,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="110" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="109" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="108" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="107" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="106" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31465,32 +31497,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="104" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="103" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="102" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="99" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31962,37 +31994,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="281" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="280" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="279" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="278" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="277" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="276" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="275" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="277" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32627,32 +32659,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="98" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="96" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="94" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="93" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33288,32 +33320,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="92" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="91" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="90" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="89" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="88" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33949,32 +33981,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="86" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="85" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="84" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="83" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="82" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34542,32 +34574,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="79" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35133,32 +35165,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="73" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35724,32 +35756,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="68" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36316,32 +36348,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="61" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="59" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36908,32 +36940,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37500,32 +37532,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38065,32 +38097,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38561,37 +38593,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="274" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="273" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="272" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="271" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="270" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="269" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="268" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39131,32 +39163,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39696,32 +39728,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40190,37 +40222,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40691,37 +40723,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41190,37 +41222,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41229,6 +41261,319 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6BDBB3-201D-44B2-9C62-F29CA02B182D}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M35" sqref="M35"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3" s="1"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4" s="1"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U30" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:C4">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0753F100-CD56-43E5-88E8-BBEB65FB07B0}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -42255,32 +42600,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="267" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="266" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="265" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="264" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="263" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="262" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42751,32 +43096,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="261" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="260" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="259" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="258" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="257" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="256" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43247,32 +43592,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="255" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="254" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="253" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="252" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="251" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="cellIs" dxfId="250" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43743,37 +44088,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="249" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="248" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="247" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="246" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="245" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="244" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="243" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44244,37 +44589,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C7 B8 A8:A9">
-    <cfRule type="cellIs" dxfId="242" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="241" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B9">
-    <cfRule type="cellIs" dxfId="240" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="239" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="238" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="cellIs" dxfId="237" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="236" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>